<commit_message>
update export report to HTML
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>TC02</t>
   </si>
@@ -26,9 +26,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Ex_AmtTotal</t>
-  </si>
-  <si>
     <t>500</t>
   </si>
   <si>
@@ -38,52 +35,10 @@
     <t>D3BE1606-A082-4A14-BC94-00B4FE38C289</t>
   </si>
   <si>
-    <t>450D658B-0DC3-4438-B86E-00B8695B3988</t>
-  </si>
-  <si>
-    <t>169F4575-BC97-49C0-A7F8-00B996BA86B7</t>
-  </si>
-  <si>
-    <t>9847DC35-9D6D-4891-BF9F-00BBBF6A5E9F</t>
-  </si>
-  <si>
-    <t>9BC68199-4AF5-4FF7-A498-00BC96BCD9B9</t>
-  </si>
-  <si>
-    <t>05700178-9B56-49E5-9CEB-00BF3EA6EC2C</t>
-  </si>
-  <si>
-    <t>8C1768B3-6990-4ACD-B48F-00C1D7A77A23</t>
-  </si>
-  <si>
-    <t>AB99D874-882A-42D2-83FA-00C3BB30D4CB</t>
-  </si>
-  <si>
-    <t>0BE6E3A8-D48A-4623-9CB3-00C6FE84DD25</t>
-  </si>
-  <si>
-    <t>54114DB8-5431-4118-A865-00C7D0A6EFCE</t>
-  </si>
-  <si>
-    <t>83309AC5-ECCF-41C9-B758-00C9DFEF1A93</t>
-  </si>
-  <si>
-    <t>396B74DC-3DAC-4276-B2C3-00CA5251154C</t>
-  </si>
-  <si>
-    <t>C803A68C-5157-4CEE-A7C0-00CFB9E5F858</t>
-  </si>
-  <si>
-    <t>F67893FB-1C51-467B-AB1B-00CFDF1782D0</t>
-  </si>
-  <si>
-    <t>EC438298-54BC-4156-95D9-00D01C580AA2</t>
-  </si>
-  <si>
-    <t>40FA0078-EA1C-4C16-A2A1-00D0870AA1BC</t>
-  </si>
-  <si>
-    <t>E3289167-5F11-4AF3-A3D7-00D3FBBE0F03</t>
+    <t>F26FD815-6AF4-4E18-B19F-009F7DC54991</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -146,14 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,24 +421,23 @@
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="30" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="30" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="N1" s="1" t="s">
+    <row r="1" spans="1:13">
+      <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -492,202 +445,37 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="D6" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="B13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="E20" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>